<commit_message>
Add versions to excel files to avoid browser caching
</commit_message>
<xml_diff>
--- a/public/excel_templates/suspended_drivers_template.xlsx
+++ b/public/excel_templates/suspended_drivers_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Front\website\public\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maden\Documents\Projects\medexams\website\public\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3DD711-9DC5-4E8F-9A77-3A2995788011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074ED4E4-66F1-4297-B55D-3B6124DA5B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Обложка" sheetId="3" r:id="rId1"/>
@@ -503,30 +503,30 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="110.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="110.6328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="20" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.77734375" style="2"/>
+    <col min="3" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="24.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
     </row>
-    <row r="8" spans="1:2" ht="275.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="275.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="16"/>
     </row>
-    <row r="11" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="20.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -534,11 +534,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -546,7 +546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
     </row>
@@ -568,26 +568,26 @@
   </sheetPr>
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="6.21875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="6.1796875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" style="11" customWidth="1"/>
     <col min="6" max="6" width="5" style="11" customWidth="1"/>
-    <col min="7" max="7" width="4.77734375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="4.81640625" style="11" customWidth="1"/>
     <col min="8" max="8" width="7" style="11" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="5.21875" style="11" customWidth="1"/>
-    <col min="11" max="12" width="7.44140625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="16.21875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="5.54296875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" style="11" customWidth="1"/>
+    <col min="11" max="12" width="7.453125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" style="11" customWidth="1"/>
     <col min="14" max="14" width="18" style="11" customWidth="1"/>
-    <col min="15" max="16384" width="12.6640625" style="11"/>
+    <col min="15" max="16384" width="12.6328125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -652,7 +652,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -672,7 +672,7 @@
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -716,7 +716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
@@ -752,7 +752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="13"/>
       <c r="C6" s="10"/>
@@ -768,7 +768,7 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -784,7 +784,7 @@
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -800,7 +800,7 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -816,7 +816,7 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -832,7 +832,7 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -848,7 +848,7 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -864,7 +864,7 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -880,7 +880,7 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -896,7 +896,7 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
     </row>
-    <row r="15" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -912,7 +912,7 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
     </row>
-    <row r="16" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -928,7 +928,7 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
     </row>
-    <row r="17" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -944,7 +944,7 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="18" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -960,7 +960,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -976,7 +976,7 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
     </row>
-    <row r="20" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -994,6 +994,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:M3"/>
@@ -1001,13 +1008,6 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1026,16 +1026,16 @@
   </sheetPr>
   <dimension ref="O45:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L40" workbookViewId="0">
+    <sheetView topLeftCell="L40" workbookViewId="0">
       <selection activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.77734375" style="8"/>
+    <col min="1" max="16384" width="8.81640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="45" spans="15:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="15:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O45" s="9" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1044,7 @@
       <c r="R45" s="9"/>
       <c r="S45" s="9"/>
     </row>
-    <row r="46" spans="15:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="15:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O46" s="9" t="s">
         <v>15</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="R46" s="9"/>
       <c r="S46" s="9"/>
     </row>
-    <row r="47" spans="15:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="15:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O47" s="9" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1062,7 @@
       <c r="R47" s="9"/>
       <c r="S47" s="9"/>
     </row>
-    <row r="48" spans="15:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="15:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O48" s="9" t="s">
         <v>17</v>
       </c>
@@ -1071,7 +1071,7 @@
       <c r="R48" s="9"/>
       <c r="S48" s="9"/>
     </row>
-    <row r="49" spans="15:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="15:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O49" s="9" t="s">
         <v>18</v>
       </c>

</xml_diff>